<commit_message>
Updated module code generator
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EO276194\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5253B137-5156-43D2-97F4-7270368B7BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73387EE-4B5F-4BF2-8033-BB9B6F43F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="25815" windowHeight="20985" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,43 +68,19 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>INTNL</t>
-  </si>
-  <si>
     <t>INTNLdata()</t>
   </si>
   <si>
-    <t>mod_Accordion_ui('INTNL_ISSS')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('INTNL_ISSS', selector=selection, data=INTNLdata(), title = c('International Student and Scholar Services'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('INTNL_ISSS', selector = selection, data = INTNLdata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</t>
-  </si>
-  <si>
     <t>International Crossroads Albany (ICA)</t>
   </si>
   <si>
-    <t>tel:(518)396-6025</t>
-  </si>
-  <si>
-    <t>https://www.icalbany.org/</t>
-  </si>
-  <si>
-    <t>mark@internationalcrossroads.org</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>ICA offers events and community for international students - primarily serves internationals at RPI, U Albany, and Union College - open to all internationals in the Capital District - activities enhance experience and understanding of American culture - includes large events, Friendship Partner Program, conversational English groups, and Bible discussions.</t>
-  </si>
-  <si>
     <t>INTNL_ICA</t>
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Email (T/F)</t>
   </si>
 </sst>
 </file>
@@ -175,7 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -189,8 +165,6 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,24 +480,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.08984375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.6328125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="27.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -542,28 +516,34 @@
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -572,7 +552,7 @@
         <v>mod_Accordion_ui('INTNL_ICA')</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -581,74 +561,38 @@
         <v>mod_Accordion_server('INTNL_ICA', selector=selection, data=INTNLdata(), title = c('International Crossroads Albany (ICA)'), Visible = T)</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
-        <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('INTNL_ICA', selector = selection, data = INTNLdata(), rownametitle = c('International Crossroads Albany (ICA)'), phone = F, website = T)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;", email = "&amp;G2&amp;")"</f>
+        <v>mod_info_server('INTNL_ICA', selector = selection, data = INTNLdata(), rownametitle = c('International Crossroads Albany (ICA)'), phone = F, website = T, email = F)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C11" s="2"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11"/>
-      <c r="G11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10"/>
+      <c r="G10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="8"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1" xr:uid="{3BCC2413-4D3D-442B-AFEC-278941669B7A}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{8C3478BC-84BB-448F-A458-7C668DAD26C4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
timely care and care training added
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EO276194\Desktop\Rolodex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandafowler/Desktop/Rolodex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73387EE-4B5F-4BF2-8033-BB9B6F43F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6829343C-373F-6345-AD7A-443F1AAF108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="25815" windowHeight="20985" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="15820" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,19 +68,28 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>INTNLdata()</t>
-  </si>
-  <si>
-    <t>International Crossroads Albany (ICA)</t>
-  </si>
-  <si>
-    <t>INTNL_ICA</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
     <t>Email (T/F)</t>
+  </si>
+  <si>
+    <t>PMH_TimelyCare</t>
+  </si>
+  <si>
+    <t>TimelyCare</t>
+  </si>
+  <si>
+    <t>PMHdata()</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('PMH_TimelyCare')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('PMH_TimelyCare', selector=selection, data=PMHdata(), title = c('TimelyCare'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('PMH_TimelyCare', selector = selection, data = PMHdata(), rownametitle = c('TimelyCare'), phone = F, website = T, email = F)</t>
   </si>
 </sst>
 </file>
@@ -482,22 +491,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="27.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -517,64 +526,67 @@
         <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('INTNL_ICA')</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>mod_Accordion_ui('PMH_TimelyCare')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('INTNL_ICA', selector=selection, data=INTNLdata(), title = c('International Crossroads Albany (ICA)'), Visible = T)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>mod_Accordion_server('PMH_TimelyCare', selector=selection, data=PMHdata(), title = c('TimelyCare'), Visible = T)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;", email = "&amp;G2&amp;")"</f>
-        <v>mod_info_server('INTNL_ICA', selector = selection, data = INTNLdata(), rownametitle = c('International Crossroads Albany (ICA)'), phone = F, website = T, email = F)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>mod_info_server('PMH_TimelyCare', selector = selection, data = PMHdata(), rownametitle = c('TimelyCare'), phone = F, website = T, email = F)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
@@ -582,13 +594,19 @@
       <c r="G10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added timely care to MHBC
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandafowler/Desktop/Rolodex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandafowler/Desktop/rolodex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6829343C-373F-6345-AD7A-443F1AAF108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5732F29F-68AF-9E42-A6BC-0B0A625E24C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="15820" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -74,22 +74,13 @@
     <t>Email (T/F)</t>
   </si>
   <si>
-    <t>PMH_TimelyCare</t>
-  </si>
-  <si>
     <t>TimelyCare</t>
   </si>
   <si>
-    <t>PMHdata()</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('PMH_TimelyCare')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('PMH_TimelyCare', selector=selection, data=PMHdata(), title = c('TimelyCare'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('PMH_TimelyCare', selector = selection, data = PMHdata(), rownametitle = c('TimelyCare'), phone = F, website = T, email = F)</t>
+    <t>BCMH_TimelyCare</t>
+  </si>
+  <si>
+    <t>MHBC()</t>
   </si>
 </sst>
 </file>
@@ -492,7 +483,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,16 +522,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -558,7 +549,7 @@
       </c>
       <c r="B4" s="1" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('PMH_TimelyCare')</v>
+        <v>mod_Accordion_ui('BCMH_TimelyCare')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -567,7 +558,7 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('PMH_TimelyCare', selector=selection, data=PMHdata(), title = c('TimelyCare'), Visible = T)</v>
+        <v>mod_Accordion_server('BCMH_TimelyCare', selector=selection, data=MHBC(), title = c('TimelyCare'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -576,7 +567,7 @@
       </c>
       <c r="B6" s="1" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;", email = "&amp;G2&amp;")"</f>
-        <v>mod_info_server('PMH_TimelyCare', selector = selection, data = PMHdata(), rownametitle = c('TimelyCare'), phone = F, website = T, email = F)</v>
+        <v>mod_info_server('BCMH_TimelyCare', selector = selection, data = MHBC(), rownametitle = c('TimelyCare'), phone = F, website = T, email = F)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -584,8 +575,9 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>15</v>
+      <c r="B10" s="1" t="str">
+        <f>"mod_Accordion_ui("&amp;"'"&amp;A8&amp;"'"&amp;")"</f>
+        <v>mod_Accordion_ui('')</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
@@ -595,14 +587,16 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>16</v>
+      <c r="B11" s="1" t="str">
+        <f>"mod_Accordion_server("&amp;"'"&amp;A8&amp;"', selector=selection, data="&amp;C8&amp;", title = c('"&amp;D8&amp;"'), Visible = T)"</f>
+        <v>mod_Accordion_server('', selector=selection, data=, title = c(''), Visible = T)</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>17</v>
+      <c r="B12" s="1" t="str">
+        <f>"mod_info_server('"&amp;A8&amp;"', selector = selection, data = "&amp;C8&amp;", rownametitle = c('"&amp;B8&amp;"'), phone = "&amp;E8&amp;", website = "&amp;F8&amp;", email = "&amp;G8&amp;")"</f>
+        <v>mod_info_server('', selector = selection, data = , rownametitle = c(''), phone = , website = , email = )</v>
       </c>
       <c r="C12" s="4"/>
     </row>

</xml_diff>

<commit_message>
added mentor, coaching, cdphp, and 211 resource
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandafowler/Desktop/rolodex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5732F29F-68AF-9E42-A6BC-0B0A625E24C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59184B6B-5942-844E-A3D3-FDA07BF629B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -74,13 +74,22 @@
     <t>Email (T/F)</t>
   </si>
   <si>
-    <t>TimelyCare</t>
-  </si>
-  <si>
-    <t>BCMH_TimelyCare</t>
-  </si>
-  <si>
-    <t>MHBC()</t>
+    <t>211 Northeast Region</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('211_NE')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('211_NE', selector=selection, data=FHFdata(), title = c('211 Northeast Region'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('211_NE', selector = selection, data = FHFdata(), rownametitle = c('211 Northeast Region'), phone = T, website = T, email = F)</t>
+  </si>
+  <si>
+    <t>211_NE_MHLC</t>
+  </si>
+  <si>
+    <t>MHLCdata()</t>
   </si>
 </sst>
 </file>
@@ -483,7 +492,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,20 +530,20 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
+      <c r="A2" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -549,7 +558,7 @@
       </c>
       <c r="B4" s="1" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('BCMH_TimelyCare')</v>
+        <v>mod_Accordion_ui('211_NE_MHLC')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -558,7 +567,7 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('BCMH_TimelyCare', selector=selection, data=MHBC(), title = c('TimelyCare'), Visible = T)</v>
+        <v>mod_Accordion_server('211_NE_MHLC', selector=selection, data=MHLCdata(), title = c('211 Northeast Region'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -567,7 +576,7 @@
       </c>
       <c r="B6" s="1" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;", email = "&amp;G2&amp;")"</f>
-        <v>mod_info_server('BCMH_TimelyCare', selector = selection, data = MHBC(), rownametitle = c('TimelyCare'), phone = F, website = T, email = F)</v>
+        <v>mod_info_server('211_NE_MHLC', selector = selection, data = MHLCdata(), rownametitle = c('211 Northeast Region'), phone = T, website = T, email = F)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -575,9 +584,8 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="str">
-        <f>"mod_Accordion_ui("&amp;"'"&amp;A8&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('')</v>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
@@ -587,16 +595,14 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="str">
-        <f>"mod_Accordion_server("&amp;"'"&amp;A8&amp;"', selector=selection, data="&amp;C8&amp;", title = c('"&amp;D8&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('', selector=selection, data=, title = c(''), Visible = T)</v>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="str">
-        <f>"mod_info_server('"&amp;A8&amp;"', selector = selection, data = "&amp;C8&amp;", rownametitle = c('"&amp;B8&amp;"'), phone = "&amp;E8&amp;", website = "&amp;F8&amp;", email = "&amp;G8&amp;")"</f>
-        <v>mod_info_server('', selector = selection, data = , rownametitle = c(''), phone = , website = , email = )</v>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C12" s="4"/>
     </row>

</xml_diff>